<commit_message>
Update spreadsheet of Daily Rainfall volumes
</commit_message>
<xml_diff>
--- a/ArchiveDocumentsSpreadsheet/DRain_Volumes.xlsx
+++ b/ArchiveDocumentsSpreadsheet/DRain_Volumes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\MetOfficeArchive\ArchiveDocumentsSpreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6B0CE-B4E3-4F67-89FA-5ADE6738FA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18293008-2306-4C0B-BCFD-C4936372281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E74CD30D-5F64-47BF-AABA-442A1BDE80E0}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="946">
   <si>
     <t>ID</t>
   </si>
@@ -1993,6 +1993,921 @@
   </si>
   <si>
     <t xml:space="preserve">1951-1962 daily rainfall for Cheshire and Lancashire </t>
+  </si>
+  <si>
+    <t>IO_216ce0cb-3280-412d-93d2-5a180ac55bb1</t>
+  </si>
+  <si>
+    <t>DRain_1922_All_Counties_Part1</t>
+  </si>
+  <si>
+    <t>IO_920a32e3-b240-46b3-9502-187dcc6f0563</t>
+  </si>
+  <si>
+    <t>DRain_1922_All_Counties_Part2</t>
+  </si>
+  <si>
+    <t>IO_9ce1201f-97dd-4cff-8fd2-fa8ce7172bf4</t>
+  </si>
+  <si>
+    <t>DRain_1923_All_Counties_Part1</t>
+  </si>
+  <si>
+    <t>IO_77f4629d-dae7-4007-833a-68a32dd7ce21</t>
+  </si>
+  <si>
+    <t>DRain_1923_All_Counties_Part2</t>
+  </si>
+  <si>
+    <t>IO_452b86c3-b0b8-4516-bca5-a44b9b52328d</t>
+  </si>
+  <si>
+    <t>DRain_1924_All_Counties_Part1</t>
+  </si>
+  <si>
+    <t>IO_7e96cf1e-536a-4486-bf5a-c049afd51841</t>
+  </si>
+  <si>
+    <t>DRain_1924_All_Counties_Part2</t>
+  </si>
+  <si>
+    <t>IO_b9b3986d-4e79-444f-8ac1-6674f3f17c1c</t>
+  </si>
+  <si>
+    <t>DRain_1925_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_233113c5-ced8-461d-83cb-2ad52048f221</t>
+  </si>
+  <si>
+    <t>DRain_1925_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_f28af379-ae9e-4e15-946b-b7861f6c6ed1</t>
+  </si>
+  <si>
+    <t>DRain_1925_Lighthouses</t>
+  </si>
+  <si>
+    <t>IO_879dcd25-a4e9-44b4-a86f-5ec3fc30f74c</t>
+  </si>
+  <si>
+    <t>DRain_1925_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_43108b2e-fd45-489e-87f4-ec644ac6796c</t>
+  </si>
+  <si>
+    <t>DRain_1925_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_c2364f9c-6410-4e0c-9ad5-2ab5e7325c86</t>
+  </si>
+  <si>
+    <t>DRain_1926_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_e3496a0f-ce89-49a5-a06e-50411c26d1a9</t>
+  </si>
+  <si>
+    <t>DRain_1926_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_5f54573b-dada-4e14-9e1e-e2107635b4ae</t>
+  </si>
+  <si>
+    <t>DRain_1926_Lighthouses</t>
+  </si>
+  <si>
+    <t>IO_3ff8a58f-b215-4145-b4c0-56fb01dbbc3d</t>
+  </si>
+  <si>
+    <t>DRain_1926_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_a0e48a71-8e28-4874-9ea0-52d6b005fe36</t>
+  </si>
+  <si>
+    <t>DRain_1926_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_adee59a6-899b-4bbe-9064-6c509192b572</t>
+  </si>
+  <si>
+    <t>DRain_1927_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_7f932bab-c896-4a90-aa55-40e95768d3e1</t>
+  </si>
+  <si>
+    <t>DRain_1927_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_ea25cbef-1627-41fa-9155-723be7589d8b</t>
+  </si>
+  <si>
+    <t>DRain_1927_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_859be26d-4381-438f-93dd-9ff770179f6a</t>
+  </si>
+  <si>
+    <t>DRain_1927_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_fd1827d6-25a3-49be-8cd0-d091d0eeb57c</t>
+  </si>
+  <si>
+    <t>DRain_1928_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_c9b93f7d-84fc-413b-a29e-9ee6ee9912e9</t>
+  </si>
+  <si>
+    <t>DRain_1928_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_3374e42a-1a83-4e79-9863-3e7d1ee5c31e</t>
+  </si>
+  <si>
+    <t>DRain_1928_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_593cb301-6000-438a-bc31-2ac3f32d13c7</t>
+  </si>
+  <si>
+    <t>DRain_1928_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_6ef3c2c0-5544-4684-a0c7-7ed9d4e101bd</t>
+  </si>
+  <si>
+    <t>DRain_1929_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_07184347-da74-489b-bd1b-20bd0e9cbde7</t>
+  </si>
+  <si>
+    <t>DRain_1929_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_69f1450e-a430-4107-bf95-c0358dd9644c</t>
+  </si>
+  <si>
+    <t>DRain_1929_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_0abdaa97-0149-4cb0-a89a-8ad13ff6432a</t>
+  </si>
+  <si>
+    <t>DRain_1929_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_9a2c3257-6667-45b9-9f50-205dd11999fa</t>
+  </si>
+  <si>
+    <t>DRain_1930_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_a7b5b246-8269-4876-b4cf-6bb72f8efe1c</t>
+  </si>
+  <si>
+    <t>DRain_1930_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_572eebb8-573a-499a-a988-30cf75dd933b</t>
+  </si>
+  <si>
+    <t>DRain_1930_Wigtown_to_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_f79e2357-1f27-40e4-bcbd-4fb3f73e861e</t>
+  </si>
+  <si>
+    <t>DRain_1930_Wigtown_to_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_a35275bd-9621-4ffa-9574-ed7a4edcb2b4</t>
+  </si>
+  <si>
+    <t>DRain_1931_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_175be60d-1705-4050-b574-af7d4e9b9cb1</t>
+  </si>
+  <si>
+    <t>DRain_1931_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_0d103d48-9e75-47a8-96fd-8bdf86f8cd4e</t>
+  </si>
+  <si>
+    <t>DRain_1931_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_743528e2-305b-4eb6-8655-62cc7bb13b1a</t>
+  </si>
+  <si>
+    <t>DRain_1931_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_65f46345-fd5b-4309-8e05-ca280979aeb2</t>
+  </si>
+  <si>
+    <t>DRain_1932_Clackmannan_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_4810d167-8aeb-4f7e-84c3-c6fcec161201</t>
+  </si>
+  <si>
+    <t>DRain_1932_Clackmannan_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_bd99af43-d359-48eb-bac0-10ed718e4c43</t>
+  </si>
+  <si>
+    <t>DRain_1932_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_f41bd671-2221-4410-8c68-2b73e656b1fd</t>
+  </si>
+  <si>
+    <t>DRain_1932_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_79eccbe6-a365-40e3-aefd-4ce30d2d4241</t>
+  </si>
+  <si>
+    <t>DRain_1933_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_5e367ad0-9f7b-47c3-8fd9-68b5590716d2</t>
+  </si>
+  <si>
+    <t>DRain_1933_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_ffd41ece-ce06-445d-af66-0bb91d862f38</t>
+  </si>
+  <si>
+    <t>DRain_1933_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_0b25e5d2-7192-4cec-a593-b78a5eb18c17</t>
+  </si>
+  <si>
+    <t>DRain_1933_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_ec87795b-c044-4502-aee6-3422aff509ca</t>
+  </si>
+  <si>
+    <t>DRain_1934_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_c0ebc7c8-481a-4620-9f93-bf723b15df66</t>
+  </si>
+  <si>
+    <t>DRain_1934_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_5b19afe1-6c0c-45f6-a33f-2e56ea4b8d5e</t>
+  </si>
+  <si>
+    <t>DRain_1934_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_3f7d8283-4384-496f-a958-49072cc74d48</t>
+  </si>
+  <si>
+    <t>DRain_1934_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_ba5100ae-4ec6-48dc-83ce-89d2d66577e4</t>
+  </si>
+  <si>
+    <t>DRain_1935_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_3bc29044-08e2-4c56-a7d4-10418aa28288</t>
+  </si>
+  <si>
+    <t>DRain_1935_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_63d59bb0-f4b6-451b-8bfd-4057a3855325</t>
+  </si>
+  <si>
+    <t>DRain_1935_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_7f27220f-8ccf-42d2-8ca7-ecbcc3a0f75a</t>
+  </si>
+  <si>
+    <t>DRain_1935_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_42a9ac71-74e8-4b97-937f-d93055e68b3a</t>
+  </si>
+  <si>
+    <t>DRain_1936_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_827ca024-d815-4675-984f-a8243a8de6df</t>
+  </si>
+  <si>
+    <t>DRain_1936_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_0e809b2a-4595-46fa-952e-6c9efc5021fb</t>
+  </si>
+  <si>
+    <t>DRain_1936_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_f868f829-093d-4f22-8434-f3f5bfcc5dc7</t>
+  </si>
+  <si>
+    <t>DRain_1936_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_9138658b-1cfd-478e-bc21-cac998fcaa49</t>
+  </si>
+  <si>
+    <t>DRain_1937_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_fc84cf2c-c0f4-49f5-89d5-58e5b78c9915</t>
+  </si>
+  <si>
+    <t>DRain_1937_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_b0e5e8cd-33b1-499e-8fc6-fa96e20e4b90</t>
+  </si>
+  <si>
+    <t>DRain_1937_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_bf2d194d-3a8c-40d5-b905-34bee3df5e8d</t>
+  </si>
+  <si>
+    <t>DRain_1937_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_53eb06e0-c80c-49e3-9daf-c0769500358f</t>
+  </si>
+  <si>
+    <t>DRain_1938_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_9bc63301-943e-4ac1-972e-e22fea5c3b6f</t>
+  </si>
+  <si>
+    <t>DRain_1938_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_d63cb368-9e6e-41bd-a703-a581148dfa48</t>
+  </si>
+  <si>
+    <t>DRain_1938_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_8dd91d53-0395-40b1-9b8b-f367e98bd111</t>
+  </si>
+  <si>
+    <t>DRain_1938_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_06bcbd3d-f925-4f0b-bf62-331336031f89</t>
+  </si>
+  <si>
+    <t>DRain_1939_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_e0102171-bb7b-4d3d-97c2-776ab40b2216</t>
+  </si>
+  <si>
+    <t>DRain_1939_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_e49b4d34-c39f-4b95-a5d3-f9e5110d8635</t>
+  </si>
+  <si>
+    <t>DRain_1939_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_dfc643e1-21e1-4c4d-b910-6c45181335ad</t>
+  </si>
+  <si>
+    <t>DRain_1939_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_c2b51642-ca28-4672-a5d0-b64692a06900</t>
+  </si>
+  <si>
+    <t>DRain_1940_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_103432e5-fbfe-49a2-8aed-eae98c429ea3</t>
+  </si>
+  <si>
+    <t>DRain_1940_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_dc4ffd3e-6e06-4011-be47-1503cf381a88</t>
+  </si>
+  <si>
+    <t>DRain_1940_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_039befd9-9181-4254-bc15-9bf5890fe6c3</t>
+  </si>
+  <si>
+    <t>DRain_1940_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_e73fecbe-bc2a-4e50-ba7d-5306ab2ad825</t>
+  </si>
+  <si>
+    <t>DRain_1941_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_2dfdd4b4-5e71-4e82-83e8-6f91a60bf581</t>
+  </si>
+  <si>
+    <t>DRain_1941_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_d8d6cca9-4ba8-4ca7-b186-af9cda8255d6</t>
+  </si>
+  <si>
+    <t>DRain_1941_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_994919c2-9060-44d6-9ee7-4be3a2989637</t>
+  </si>
+  <si>
+    <t>DRain_1941_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_060d834d-540e-4f61-97bf-19a877530db4</t>
+  </si>
+  <si>
+    <t>DRain_1942_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_ebd796cc-a520-422f-9120-4b49f651d5f9</t>
+  </si>
+  <si>
+    <t>DRain_1942_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_d7ba1895-c979-409a-99f2-2e3beff261d0</t>
+  </si>
+  <si>
+    <t>DRain_1942_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_c3168798-8bf2-4954-8063-fab948076ed5</t>
+  </si>
+  <si>
+    <t>DRain_1942_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_b20e3f50-d118-4e13-8ce8-be832ff5709e</t>
+  </si>
+  <si>
+    <t>DRain_1943_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_57b4bc71-769d-4db4-9b31-ff1bb9b34199</t>
+  </si>
+  <si>
+    <t>DRain_1943_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_2f7845bf-4303-4f7e-8be1-a9a66a62ee90</t>
+  </si>
+  <si>
+    <t>DRain_1943_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_40c739ff-a556-4711-851e-f77bc85f8314</t>
+  </si>
+  <si>
+    <t>DRain_1943_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_ab1fd4c6-0cfd-44de-a52c-f833fe60f58e</t>
+  </si>
+  <si>
+    <t>DRain_1944_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_8aabd472-236c-487a-801a-10f7738951a4</t>
+  </si>
+  <si>
+    <t>DRain_1944_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_6e7e3a38-a8e6-45cf-97f9-7b4d753161ec</t>
+  </si>
+  <si>
+    <t>DRain_1944_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_7864b6ed-ac5c-4fb4-b8ec-71dd4f779f47</t>
+  </si>
+  <si>
+    <t>DRain_1944_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_d1e1966b-c2e9-4996-b208-962f346cb7a4</t>
+  </si>
+  <si>
+    <t>DRain_1945_Clackmannan_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_7a640056-ecde-4daf-9e07-61e3e5d85413</t>
+  </si>
+  <si>
+    <t>DRain_1945_Clackmannan_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_eb9bdda4-211d-4be3-ba6f-4662b8c8b257</t>
+  </si>
+  <si>
+    <t>DRain_1945_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_56553ec5-0bd4-4d60-9e27-81b1607dc1a8</t>
+  </si>
+  <si>
+    <t>DRain_1945_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_a1b6ddbb-6d07-4de5-bc0a-1e5030c2d25c</t>
+  </si>
+  <si>
+    <t>DRain_1946_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_fbdd17f2-b636-45c5-9cd5-190bca09bb5c</t>
+  </si>
+  <si>
+    <t>DRain_1946_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_c8e1baaf-e739-4712-a8ab-63c2238290e3</t>
+  </si>
+  <si>
+    <t>DRain_1946_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_264abd63-cfb2-4f35-831f-622e5ae153f3</t>
+  </si>
+  <si>
+    <t>DRain_1946_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_0e28d4c1-4c88-4bcd-bb1a-1edc590be098</t>
+  </si>
+  <si>
+    <t>DRain_1947_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_7d4113c4-4634-448d-be7d-baed0b03010f</t>
+  </si>
+  <si>
+    <t>DRain_1947_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_21f9621d-8e40-44ab-8c6e-84d98bdb493f</t>
+  </si>
+  <si>
+    <t>DRain_1947_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_f20337eb-4941-4cae-b260-d512b7cc4cca</t>
+  </si>
+  <si>
+    <t>DRain_1947_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_b7d1d78a-0ca6-4e61-acf0-b102a06cb436</t>
+  </si>
+  <si>
+    <t>DRain_1948_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_b60eb0be-e260-4054-8ad4-7d3b5bf3d033</t>
+  </si>
+  <si>
+    <t>DRain_1948_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_c272976b-421f-4eaa-a291-ee546244e555</t>
+  </si>
+  <si>
+    <t>DRain_1948_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_ca87e296-bbfd-4d0f-aede-2e70c3b96aea</t>
+  </si>
+  <si>
+    <t>DRain_1948_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_56ddea0d-09a3-45e4-a6b7-e0706cf9ebfe</t>
+  </si>
+  <si>
+    <t>DRain_1949_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_f0e6aba9-7bcb-4130-90f0-bc69574e2d6e</t>
+  </si>
+  <si>
+    <t>DRain_1949_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_e510d805-c82c-4f95-90a1-3913efdbd328</t>
+  </si>
+  <si>
+    <t>DRain_1949_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_012aecb1-3bcf-443d-b44f-5ddda7c26c8a</t>
+  </si>
+  <si>
+    <t>DRain_1949_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_fdc7d74b-ca7a-44bb-8a3e-88adbfef8fd6</t>
+  </si>
+  <si>
+    <t>DRain_1950_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_3bb146f2-8e6d-4603-839d-3c77a688f3a0</t>
+  </si>
+  <si>
+    <t>DRain_1950_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_65268de4-07c2-47be-8865-b33f45ee5b98</t>
+  </si>
+  <si>
+    <t>DRain_1950_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_47046fca-1a78-4b33-a26c-de0a02e8cc7c</t>
+  </si>
+  <si>
+    <t>DRain_1950_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_538a1fbd-3b8e-4f63-8515-cbcd11cc9459</t>
+  </si>
+  <si>
+    <t>DRain_1951_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_d4658066-6a31-453c-874a-5367431cfb5f</t>
+  </si>
+  <si>
+    <t>DRain_1951_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_cf6bc6a7-e17a-425f-b1e7-bf45ae4bf6bd</t>
+  </si>
+  <si>
+    <t>DRain_1951_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_ad16a96b-82ca-4885-b5bf-2bcbd2833328</t>
+  </si>
+  <si>
+    <t>DRain_1951_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_5e146fdb-db64-4975-87ff-6eb58f8c2359</t>
+  </si>
+  <si>
+    <t>DRain_1952_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_f01db020-b79b-490c-a3dd-8640fc3e1e64</t>
+  </si>
+  <si>
+    <t>DRain_1952_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_4241e839-7b68-4aab-b50d-219e286010ef</t>
+  </si>
+  <si>
+    <t>DRain_1952_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_9770d279-ede9-4f63-9d38-02ca6e67bdc8</t>
+  </si>
+  <si>
+    <t>DRain_1952_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_2b20ccbf-9a2b-4663-abbe-5a239fa516b3</t>
+  </si>
+  <si>
+    <t>DRain_1953_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_d8d80656-bd9b-4adc-9ccc-903c8a6ceb21</t>
+  </si>
+  <si>
+    <t>DRain_1953_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_9e42794a-dd8c-467c-a4a3-8183cbc59935</t>
+  </si>
+  <si>
+    <t>DRain_1953_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_d03eddd5-0499-47cc-a96b-a9d127b9a70f</t>
+  </si>
+  <si>
+    <t>DRain_1953_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_23c384da-07c7-4751-a5f6-4dbb6eaa0fd5</t>
+  </si>
+  <si>
+    <t>DRain_1954_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_f13a8774-f853-4a77-9ef0-a29e5bd93cc7</t>
+  </si>
+  <si>
+    <t>DRain_1954_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_908c45a3-d106-4440-b1a2-8c077edf052d</t>
+  </si>
+  <si>
+    <t>DRain_1954_Wigtown_to_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_e9cf4c0a-b740-4ddc-bb99-b3bb093b8ca2</t>
+  </si>
+  <si>
+    <t>DRain_1954_Wigtown_to_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_eb0bdc4e-7089-44af-8788-fb449af3cf0a</t>
+  </si>
+  <si>
+    <t>DRain_1955_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_ffc3e578-ca17-4d29-af32-f6bd2b5aaa8d</t>
+  </si>
+  <si>
+    <t>DRain_1955_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_005b2e6b-b329-4af0-9f96-ac93ee12f6c0</t>
+  </si>
+  <si>
+    <t>DRain_1955_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_88d2bb3f-12d8-4739-8a22-41bda4de45ef</t>
+  </si>
+  <si>
+    <t>DRain_1955_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_093f3eae-cb3f-4fa9-8209-2b9daa531a0d</t>
+  </si>
+  <si>
+    <t>DRain_1956_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_a5f48195-3af1-48ee-a31f-6341f501ed35</t>
+  </si>
+  <si>
+    <t>DRain_1956_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_10ec839a-937e-4ca4-be03-4ab8d579b981</t>
+  </si>
+  <si>
+    <t>DRain_1956_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_ad8f12d0-8062-4370-b393-129121a9fb8d</t>
+  </si>
+  <si>
+    <t>DRain_1956_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_f1eea438-669d-43f9-b3e1-dd08aa744bdf</t>
+  </si>
+  <si>
+    <t>DRain_1957_Clackmannan_to_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_a5d587e2-372e-4010-8868-4c87155096c9</t>
+  </si>
+  <si>
+    <t>DRain_1957_Clackmannan_to_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_49a0acfb-d5b8-4602-ba8b-5ad42de5cb29</t>
+  </si>
+  <si>
+    <t>DRain_1957_Wigtown_to_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_43fb04d3-3b67-482c-ac58-66254b341e6e</t>
+  </si>
+  <si>
+    <t>DRain_1957_Wigtown_to_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_32d6d512-3187-45e2-a2dc-66e27cc0ce9b</t>
+  </si>
+  <si>
+    <t>DRain_1958_Clackmannan_to_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_99d077bb-129e-42b7-b1a7-ac4bc5a17a02</t>
+  </si>
+  <si>
+    <t>DRain_1958_Clackmannan_to_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_ad6d3338-a490-407b-bf2a-4156d16cb72c</t>
+  </si>
+  <si>
+    <t>DRain_1958_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_01afc75e-6cad-4a36-9f11-b1608e2ca2ca</t>
+  </si>
+  <si>
+    <t>DRain_1958_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_990db1a6-8c3d-418e-8701-cdeb48abc8dd</t>
+  </si>
+  <si>
+    <t>DRain_1959_Clackmannan_to_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_a13cc31a-b3ce-44bf-8dfa-826dc8b2dd19</t>
+  </si>
+  <si>
+    <t>DRain_1959_Clackmannan_to_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_fce53910-5eb7-4ee2-b6af-c49b9750ab08</t>
+  </si>
+  <si>
+    <t>DRain_1959_Wigtown_To_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_0b3d18a7-4593-4a28-a48f-c861e2ded78a</t>
+  </si>
+  <si>
+    <t>DRain_1959_Wigtown_To_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>IO_7d8b8e31-18a8-406e-ad35-cdc06e932f72</t>
+  </si>
+  <si>
+    <t>DRain_1960_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>IO_d0e6f9c2-34bd-489b-9a5e-f6d658c5f1f2</t>
+  </si>
+  <si>
+    <t>DRain_1960_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>IO_e4ed6f38-7efb-47c8-a26e-8a9583cb4c7d</t>
+  </si>
+  <si>
+    <t>DRain_1960_Wigtown_to_Argyll_Part1</t>
+  </si>
+  <si>
+    <t>IO_302f9c91-2b83-4094-96ea-7cf6dfff3034</t>
+  </si>
+  <si>
+    <t>DRain_1960_Wigtown_to_Argyll_Part2</t>
+  </si>
+  <si>
+    <t>[Scotland]</t>
   </si>
 </sst>
 </file>
@@ -2867,17 +3782,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5949EA17-9A17-41A4-8A1A-605F6AA36F9B}">
-  <dimension ref="A1:C241"/>
+  <dimension ref="A1:C393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C215" sqref="C215"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5532,6 +6447,1678 @@
         <v>627</v>
       </c>
     </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>641</v>
+      </c>
+      <c r="B242" t="s">
+        <v>642</v>
+      </c>
+      <c r="C242" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>643</v>
+      </c>
+      <c r="B243" t="s">
+        <v>644</v>
+      </c>
+      <c r="C243" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>645</v>
+      </c>
+      <c r="B244" t="s">
+        <v>646</v>
+      </c>
+      <c r="C244" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>647</v>
+      </c>
+      <c r="B245" t="s">
+        <v>648</v>
+      </c>
+      <c r="C245" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>649</v>
+      </c>
+      <c r="B246" t="s">
+        <v>650</v>
+      </c>
+      <c r="C246" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>651</v>
+      </c>
+      <c r="B247" t="s">
+        <v>652</v>
+      </c>
+      <c r="C247" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>653</v>
+      </c>
+      <c r="B248" t="s">
+        <v>654</v>
+      </c>
+      <c r="C248" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>655</v>
+      </c>
+      <c r="B249" t="s">
+        <v>656</v>
+      </c>
+      <c r="C249" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>657</v>
+      </c>
+      <c r="B250" t="s">
+        <v>658</v>
+      </c>
+      <c r="C250" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>659</v>
+      </c>
+      <c r="B251" t="s">
+        <v>660</v>
+      </c>
+      <c r="C251" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>661</v>
+      </c>
+      <c r="B252" t="s">
+        <v>662</v>
+      </c>
+      <c r="C252" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>663</v>
+      </c>
+      <c r="B253" t="s">
+        <v>664</v>
+      </c>
+      <c r="C253" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>665</v>
+      </c>
+      <c r="B254" t="s">
+        <v>666</v>
+      </c>
+      <c r="C254" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>667</v>
+      </c>
+      <c r="B255" t="s">
+        <v>668</v>
+      </c>
+      <c r="C255" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>669</v>
+      </c>
+      <c r="B256" t="s">
+        <v>670</v>
+      </c>
+      <c r="C256" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>671</v>
+      </c>
+      <c r="B257" t="s">
+        <v>672</v>
+      </c>
+      <c r="C257" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>673</v>
+      </c>
+      <c r="B258" t="s">
+        <v>674</v>
+      </c>
+      <c r="C258" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>675</v>
+      </c>
+      <c r="B259" t="s">
+        <v>676</v>
+      </c>
+      <c r="C259" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>677</v>
+      </c>
+      <c r="B260" t="s">
+        <v>678</v>
+      </c>
+      <c r="C260" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>679</v>
+      </c>
+      <c r="B261" t="s">
+        <v>680</v>
+      </c>
+      <c r="C261" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>681</v>
+      </c>
+      <c r="B262" t="s">
+        <v>682</v>
+      </c>
+      <c r="C262" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>683</v>
+      </c>
+      <c r="B263" t="s">
+        <v>684</v>
+      </c>
+      <c r="C263" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>685</v>
+      </c>
+      <c r="B264" t="s">
+        <v>686</v>
+      </c>
+      <c r="C264" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>687</v>
+      </c>
+      <c r="B265" t="s">
+        <v>688</v>
+      </c>
+      <c r="C265" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>689</v>
+      </c>
+      <c r="B266" t="s">
+        <v>690</v>
+      </c>
+      <c r="C266" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>691</v>
+      </c>
+      <c r="B267" t="s">
+        <v>692</v>
+      </c>
+      <c r="C267" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>693</v>
+      </c>
+      <c r="B268" t="s">
+        <v>694</v>
+      </c>
+      <c r="C268" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>695</v>
+      </c>
+      <c r="B269" t="s">
+        <v>696</v>
+      </c>
+      <c r="C269" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>697</v>
+      </c>
+      <c r="B270" t="s">
+        <v>698</v>
+      </c>
+      <c r="C270" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>699</v>
+      </c>
+      <c r="B271" t="s">
+        <v>700</v>
+      </c>
+      <c r="C271" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>701</v>
+      </c>
+      <c r="B272" t="s">
+        <v>702</v>
+      </c>
+      <c r="C272" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>703</v>
+      </c>
+      <c r="B273" t="s">
+        <v>704</v>
+      </c>
+      <c r="C273" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>705</v>
+      </c>
+      <c r="B274" t="s">
+        <v>706</v>
+      </c>
+      <c r="C274" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>707</v>
+      </c>
+      <c r="B275" t="s">
+        <v>708</v>
+      </c>
+      <c r="C275" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>709</v>
+      </c>
+      <c r="B276" t="s">
+        <v>710</v>
+      </c>
+      <c r="C276" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>711</v>
+      </c>
+      <c r="B277" t="s">
+        <v>712</v>
+      </c>
+      <c r="C277" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>713</v>
+      </c>
+      <c r="B278" t="s">
+        <v>714</v>
+      </c>
+      <c r="C278" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>715</v>
+      </c>
+      <c r="B279" t="s">
+        <v>716</v>
+      </c>
+      <c r="C279" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>717</v>
+      </c>
+      <c r="B280" t="s">
+        <v>718</v>
+      </c>
+      <c r="C280" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>719</v>
+      </c>
+      <c r="B281" t="s">
+        <v>720</v>
+      </c>
+      <c r="C281" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>721</v>
+      </c>
+      <c r="B282" t="s">
+        <v>722</v>
+      </c>
+      <c r="C282" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>723</v>
+      </c>
+      <c r="B283" t="s">
+        <v>724</v>
+      </c>
+      <c r="C283" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>725</v>
+      </c>
+      <c r="B284" t="s">
+        <v>726</v>
+      </c>
+      <c r="C284" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>727</v>
+      </c>
+      <c r="B285" t="s">
+        <v>728</v>
+      </c>
+      <c r="C285" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>729</v>
+      </c>
+      <c r="B286" t="s">
+        <v>730</v>
+      </c>
+      <c r="C286" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>731</v>
+      </c>
+      <c r="B287" t="s">
+        <v>732</v>
+      </c>
+      <c r="C287" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>733</v>
+      </c>
+      <c r="B288" t="s">
+        <v>734</v>
+      </c>
+      <c r="C288" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>735</v>
+      </c>
+      <c r="B289" t="s">
+        <v>736</v>
+      </c>
+      <c r="C289" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>737</v>
+      </c>
+      <c r="B290" t="s">
+        <v>738</v>
+      </c>
+      <c r="C290" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>739</v>
+      </c>
+      <c r="B291" t="s">
+        <v>740</v>
+      </c>
+      <c r="C291" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>741</v>
+      </c>
+      <c r="B292" t="s">
+        <v>742</v>
+      </c>
+      <c r="C292" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>743</v>
+      </c>
+      <c r="B293" t="s">
+        <v>744</v>
+      </c>
+      <c r="C293" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>745</v>
+      </c>
+      <c r="B294" t="s">
+        <v>746</v>
+      </c>
+      <c r="C294" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>747</v>
+      </c>
+      <c r="B295" t="s">
+        <v>748</v>
+      </c>
+      <c r="C295" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>749</v>
+      </c>
+      <c r="B296" t="s">
+        <v>750</v>
+      </c>
+      <c r="C296" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>751</v>
+      </c>
+      <c r="B297" t="s">
+        <v>752</v>
+      </c>
+      <c r="C297" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>753</v>
+      </c>
+      <c r="B298" t="s">
+        <v>754</v>
+      </c>
+      <c r="C298" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>755</v>
+      </c>
+      <c r="B299" t="s">
+        <v>756</v>
+      </c>
+      <c r="C299" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>757</v>
+      </c>
+      <c r="B300" t="s">
+        <v>758</v>
+      </c>
+      <c r="C300" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>759</v>
+      </c>
+      <c r="B301" t="s">
+        <v>760</v>
+      </c>
+      <c r="C301" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>761</v>
+      </c>
+      <c r="B302" t="s">
+        <v>762</v>
+      </c>
+      <c r="C302" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>763</v>
+      </c>
+      <c r="B303" t="s">
+        <v>764</v>
+      </c>
+      <c r="C303" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>765</v>
+      </c>
+      <c r="B304" t="s">
+        <v>766</v>
+      </c>
+      <c r="C304" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>767</v>
+      </c>
+      <c r="B305" t="s">
+        <v>768</v>
+      </c>
+      <c r="C305" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>769</v>
+      </c>
+      <c r="B306" t="s">
+        <v>770</v>
+      </c>
+      <c r="C306" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>771</v>
+      </c>
+      <c r="B307" t="s">
+        <v>772</v>
+      </c>
+      <c r="C307" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>773</v>
+      </c>
+      <c r="B308" t="s">
+        <v>774</v>
+      </c>
+      <c r="C308" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>775</v>
+      </c>
+      <c r="B309" t="s">
+        <v>776</v>
+      </c>
+      <c r="C309" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>777</v>
+      </c>
+      <c r="B310" t="s">
+        <v>778</v>
+      </c>
+      <c r="C310" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>779</v>
+      </c>
+      <c r="B311" t="s">
+        <v>780</v>
+      </c>
+      <c r="C311" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>781</v>
+      </c>
+      <c r="B312" t="s">
+        <v>782</v>
+      </c>
+      <c r="C312" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>783</v>
+      </c>
+      <c r="B313" t="s">
+        <v>784</v>
+      </c>
+      <c r="C313" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>785</v>
+      </c>
+      <c r="B314" t="s">
+        <v>786</v>
+      </c>
+      <c r="C314" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>787</v>
+      </c>
+      <c r="B315" t="s">
+        <v>788</v>
+      </c>
+      <c r="C315" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>789</v>
+      </c>
+      <c r="B316" t="s">
+        <v>790</v>
+      </c>
+      <c r="C316" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>791</v>
+      </c>
+      <c r="B317" t="s">
+        <v>792</v>
+      </c>
+      <c r="C317" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>793</v>
+      </c>
+      <c r="B318" t="s">
+        <v>794</v>
+      </c>
+      <c r="C318" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>795</v>
+      </c>
+      <c r="B319" t="s">
+        <v>796</v>
+      </c>
+      <c r="C319" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>797</v>
+      </c>
+      <c r="B320" t="s">
+        <v>798</v>
+      </c>
+      <c r="C320" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>799</v>
+      </c>
+      <c r="B321" t="s">
+        <v>800</v>
+      </c>
+      <c r="C321" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>801</v>
+      </c>
+      <c r="B322" t="s">
+        <v>802</v>
+      </c>
+      <c r="C322" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>803</v>
+      </c>
+      <c r="B323" t="s">
+        <v>804</v>
+      </c>
+      <c r="C323" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>805</v>
+      </c>
+      <c r="B324" t="s">
+        <v>806</v>
+      </c>
+      <c r="C324" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>807</v>
+      </c>
+      <c r="B325" t="s">
+        <v>808</v>
+      </c>
+      <c r="C325" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>809</v>
+      </c>
+      <c r="B326" t="s">
+        <v>810</v>
+      </c>
+      <c r="C326" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>811</v>
+      </c>
+      <c r="B327" t="s">
+        <v>812</v>
+      </c>
+      <c r="C327" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>813</v>
+      </c>
+      <c r="B328" t="s">
+        <v>814</v>
+      </c>
+      <c r="C328" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>815</v>
+      </c>
+      <c r="B329" t="s">
+        <v>816</v>
+      </c>
+      <c r="C329" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>817</v>
+      </c>
+      <c r="B330" t="s">
+        <v>818</v>
+      </c>
+      <c r="C330" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>819</v>
+      </c>
+      <c r="B331" t="s">
+        <v>820</v>
+      </c>
+      <c r="C331" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>821</v>
+      </c>
+      <c r="B332" t="s">
+        <v>822</v>
+      </c>
+      <c r="C332" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>823</v>
+      </c>
+      <c r="B333" t="s">
+        <v>824</v>
+      </c>
+      <c r="C333" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>825</v>
+      </c>
+      <c r="B334" t="s">
+        <v>826</v>
+      </c>
+      <c r="C334" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>827</v>
+      </c>
+      <c r="B335" t="s">
+        <v>828</v>
+      </c>
+      <c r="C335" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>829</v>
+      </c>
+      <c r="B336" t="s">
+        <v>830</v>
+      </c>
+      <c r="C336" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>831</v>
+      </c>
+      <c r="B337" t="s">
+        <v>832</v>
+      </c>
+      <c r="C337" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>833</v>
+      </c>
+      <c r="B338" t="s">
+        <v>834</v>
+      </c>
+      <c r="C338" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>835</v>
+      </c>
+      <c r="B339" t="s">
+        <v>836</v>
+      </c>
+      <c r="C339" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>837</v>
+      </c>
+      <c r="B340" t="s">
+        <v>838</v>
+      </c>
+      <c r="C340" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>839</v>
+      </c>
+      <c r="B341" t="s">
+        <v>840</v>
+      </c>
+      <c r="C341" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>841</v>
+      </c>
+      <c r="B342" t="s">
+        <v>842</v>
+      </c>
+      <c r="C342" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>843</v>
+      </c>
+      <c r="B343" t="s">
+        <v>844</v>
+      </c>
+      <c r="C343" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>845</v>
+      </c>
+      <c r="B344" t="s">
+        <v>846</v>
+      </c>
+      <c r="C344" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>847</v>
+      </c>
+      <c r="B345" t="s">
+        <v>848</v>
+      </c>
+      <c r="C345" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>849</v>
+      </c>
+      <c r="B346" t="s">
+        <v>850</v>
+      </c>
+      <c r="C346" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>851</v>
+      </c>
+      <c r="B347" t="s">
+        <v>852</v>
+      </c>
+      <c r="C347" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>853</v>
+      </c>
+      <c r="B348" t="s">
+        <v>854</v>
+      </c>
+      <c r="C348" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>855</v>
+      </c>
+      <c r="B349" t="s">
+        <v>856</v>
+      </c>
+      <c r="C349" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>857</v>
+      </c>
+      <c r="B350" t="s">
+        <v>858</v>
+      </c>
+      <c r="C350" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>859</v>
+      </c>
+      <c r="B351" t="s">
+        <v>860</v>
+      </c>
+      <c r="C351" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>861</v>
+      </c>
+      <c r="B352" t="s">
+        <v>862</v>
+      </c>
+      <c r="C352" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>863</v>
+      </c>
+      <c r="B353" t="s">
+        <v>864</v>
+      </c>
+      <c r="C353" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>865</v>
+      </c>
+      <c r="B354" t="s">
+        <v>866</v>
+      </c>
+      <c r="C354" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>867</v>
+      </c>
+      <c r="B355" t="s">
+        <v>868</v>
+      </c>
+      <c r="C355" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>869</v>
+      </c>
+      <c r="B356" t="s">
+        <v>870</v>
+      </c>
+      <c r="C356" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>871</v>
+      </c>
+      <c r="B357" t="s">
+        <v>872</v>
+      </c>
+      <c r="C357" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>873</v>
+      </c>
+      <c r="B358" t="s">
+        <v>874</v>
+      </c>
+      <c r="C358" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>875</v>
+      </c>
+      <c r="B359" t="s">
+        <v>876</v>
+      </c>
+      <c r="C359" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>877</v>
+      </c>
+      <c r="B360" t="s">
+        <v>878</v>
+      </c>
+      <c r="C360" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>879</v>
+      </c>
+      <c r="B361" t="s">
+        <v>880</v>
+      </c>
+      <c r="C361" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>881</v>
+      </c>
+      <c r="B362" t="s">
+        <v>882</v>
+      </c>
+      <c r="C362" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>883</v>
+      </c>
+      <c r="B363" t="s">
+        <v>884</v>
+      </c>
+      <c r="C363" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>885</v>
+      </c>
+      <c r="B364" t="s">
+        <v>886</v>
+      </c>
+      <c r="C364" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>887</v>
+      </c>
+      <c r="B365" t="s">
+        <v>888</v>
+      </c>
+      <c r="C365" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>889</v>
+      </c>
+      <c r="B366" t="s">
+        <v>890</v>
+      </c>
+      <c r="C366" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>891</v>
+      </c>
+      <c r="B367" t="s">
+        <v>892</v>
+      </c>
+      <c r="C367" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>893</v>
+      </c>
+      <c r="B368" t="s">
+        <v>894</v>
+      </c>
+      <c r="C368" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>895</v>
+      </c>
+      <c r="B369" t="s">
+        <v>896</v>
+      </c>
+      <c r="C369" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>897</v>
+      </c>
+      <c r="B370" t="s">
+        <v>898</v>
+      </c>
+      <c r="C370" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>899</v>
+      </c>
+      <c r="B371" t="s">
+        <v>900</v>
+      </c>
+      <c r="C371" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>901</v>
+      </c>
+      <c r="B372" t="s">
+        <v>902</v>
+      </c>
+      <c r="C372" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>903</v>
+      </c>
+      <c r="B373" t="s">
+        <v>904</v>
+      </c>
+      <c r="C373" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>905</v>
+      </c>
+      <c r="B374" t="s">
+        <v>906</v>
+      </c>
+      <c r="C374" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>907</v>
+      </c>
+      <c r="B375" t="s">
+        <v>908</v>
+      </c>
+      <c r="C375" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>909</v>
+      </c>
+      <c r="B376" t="s">
+        <v>910</v>
+      </c>
+      <c r="C376" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>911</v>
+      </c>
+      <c r="B377" t="s">
+        <v>912</v>
+      </c>
+      <c r="C377" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>913</v>
+      </c>
+      <c r="B378" t="s">
+        <v>914</v>
+      </c>
+      <c r="C378" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>915</v>
+      </c>
+      <c r="B379" t="s">
+        <v>916</v>
+      </c>
+      <c r="C379" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>917</v>
+      </c>
+      <c r="B380" t="s">
+        <v>918</v>
+      </c>
+      <c r="C380" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>919</v>
+      </c>
+      <c r="B381" t="s">
+        <v>920</v>
+      </c>
+      <c r="C381" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>921</v>
+      </c>
+      <c r="B382" t="s">
+        <v>922</v>
+      </c>
+      <c r="C382" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>923</v>
+      </c>
+      <c r="B383" t="s">
+        <v>924</v>
+      </c>
+      <c r="C383" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>925</v>
+      </c>
+      <c r="B384" t="s">
+        <v>926</v>
+      </c>
+      <c r="C384" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>927</v>
+      </c>
+      <c r="B385" t="s">
+        <v>928</v>
+      </c>
+      <c r="C385" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>929</v>
+      </c>
+      <c r="B386" t="s">
+        <v>930</v>
+      </c>
+      <c r="C386" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>931</v>
+      </c>
+      <c r="B387" t="s">
+        <v>932</v>
+      </c>
+      <c r="C387" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>933</v>
+      </c>
+      <c r="B388" t="s">
+        <v>934</v>
+      </c>
+      <c r="C388" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>935</v>
+      </c>
+      <c r="B389" t="s">
+        <v>936</v>
+      </c>
+      <c r="C389" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>937</v>
+      </c>
+      <c r="B390" t="s">
+        <v>938</v>
+      </c>
+      <c r="C390" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>939</v>
+      </c>
+      <c r="B391" t="s">
+        <v>940</v>
+      </c>
+      <c r="C391" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>941</v>
+      </c>
+      <c r="B392" t="s">
+        <v>942</v>
+      </c>
+      <c r="C392" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>943</v>
+      </c>
+      <c r="B393" t="s">
+        <v>944</v>
+      </c>
+      <c r="C393" t="s">
+        <v>945</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C241" xr:uid="{5949EA17-9A17-41A4-8A1A-605F6AA36F9B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Partial refresh of Met Office Archive spreadsheet with latest Daily Rainfall volumes
</commit_message>
<xml_diff>
--- a/ArchiveDocumentsSpreadsheet/DRain_Volumes.xlsx
+++ b/ArchiveDocumentsSpreadsheet/DRain_Volumes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\MetOfficeArchive\ArchiveDocumentsSpreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18293008-2306-4C0B-BCFD-C4936372281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242C989C-D35F-402C-BA05-76CF5514941D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E74CD30D-5F64-47BF-AABA-442A1BDE80E0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Drain" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drain!$A$1:$C$241</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drain!$A$1:$C$523</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,12 +65,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{7CEFC09D-AC8A-4BB8-AC99-AAA6B3C8A915}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Met Office Online Archive description</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="1286">
   <si>
     <t>ID</t>
   </si>
@@ -2908,6 +2932,1026 @@
   </si>
   <si>
     <t>[Scotland]</t>
+  </si>
+  <si>
+    <t>IO_bcfaed16-b5ae-4746-8491-1ba91e40ac18</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0001-0050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for London </t>
+  </si>
+  <si>
+    <t>IO_8e2b427d-4e7d-4f40-b2fb-2bd88ebee94a</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0051-0069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for London and Surrey </t>
+  </si>
+  <si>
+    <t>IO_ff4247c7-7e35-4f63-8494-8c8f032a8554</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0070-0100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Surrey </t>
+  </si>
+  <si>
+    <t>IO_f241c4f6-157a-46d6-abb4-52ea5b0927a0</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0100-0133</t>
+  </si>
+  <si>
+    <t>IO_12d6f32f-75e6-43a9-8f88-07bbadaa4241</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0133-0150</t>
+  </si>
+  <si>
+    <t>IO_e4156a2a-08e0-4744-b03e-b515cd161d23</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0151-0180</t>
+  </si>
+  <si>
+    <t>IO_79d4fbc6-95e4-4d25-a0b9-ed4316d4d182</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0181-0199</t>
+  </si>
+  <si>
+    <t>IO_342b37d1-157c-4b95-aca0-198c9e773fcc</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0200-0225</t>
+  </si>
+  <si>
+    <t>IO_1d94aa20-e356-4da4-8174-d2611cf14035</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0226-0250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Surrey and Kent </t>
+  </si>
+  <si>
+    <t>IO_a33be3b3-ae9f-4441-b93a-6b55c1248170</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0250-0285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Kent </t>
+  </si>
+  <si>
+    <t>IO_0972fb1f-eac4-4a1c-be60-3d3f67d0339d</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0286-0315</t>
+  </si>
+  <si>
+    <t>IO_a7960839-7d27-4a7f-ab04-180a1c8cb70e</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0316-0350</t>
+  </si>
+  <si>
+    <t>IO_92e0a4c2-3a71-45a7-8fd5-562758aa08db</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0351-0391</t>
+  </si>
+  <si>
+    <t>IO_5ee8b91c-a648-4eb6-a430-34aa6d3703eb</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0392-0419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Kent and Sussex </t>
+  </si>
+  <si>
+    <t>IO_a4748ef5-6894-4160-9d65-67f71ba53cd6</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0420-0450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Sussex </t>
+  </si>
+  <si>
+    <t>IO_b5270954-42cf-4011-819f-bee4c3254089</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0451-0472</t>
+  </si>
+  <si>
+    <t>IO_26d42a08-9f54-438f-897c-a510f15cd977</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0473-0510</t>
+  </si>
+  <si>
+    <t>IO_aba0a6c2-1edf-4200-bc10-0b814565bedf</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0511-0545</t>
+  </si>
+  <si>
+    <t>IO_09df6b66-6d7c-49f8-af61-e47d410f2679</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0546-0572</t>
+  </si>
+  <si>
+    <t>IO_262e7020-6c48-4d84-908d-7815d1f81074</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0573-0611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Sussex and Hampshire </t>
+  </si>
+  <si>
+    <t>IO_8a0a8d8e-2cab-4a7a-8ec0-58c04b0be2d8</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0612-0642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Hampshire </t>
+  </si>
+  <si>
+    <t>IO_0717b4ec-3dcf-40a2-b45b-e7f901359685</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0643-0678</t>
+  </si>
+  <si>
+    <t>IO_4c5d9e75-eb90-44d8-b636-5c5d08f68994</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0679-0717</t>
+  </si>
+  <si>
+    <t>IO_df546115-3ade-4cdd-8d02-67983648552c</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0718-0750</t>
+  </si>
+  <si>
+    <t>IO_beea6117-4db3-4453-bce9-20041e4a8120</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0751-0780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Hampshire and Berkshire </t>
+  </si>
+  <si>
+    <t>IO_2df96d5a-c9e0-43ac-a4af-ab856c5595fa</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0781-0810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Berkshire </t>
+  </si>
+  <si>
+    <t>IO_cab95a77-9515-4d2b-8ef8-87dcb90faa00</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0811-0845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Berkshire and Middlesex </t>
+  </si>
+  <si>
+    <t>IO_9c7c28f4-61d8-4061-964d-20c88365da29</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0846-0875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Middlesex and Hertfordshire </t>
+  </si>
+  <si>
+    <t>IO_5cbca0d0-37a1-4f8a-af95-6917a12f35a0</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0876-0900</t>
+  </si>
+  <si>
+    <t>IO_259dd7f8-13f6-4f09-8bdd-487f795182c0</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0901-0937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Hertfordshire </t>
+  </si>
+  <si>
+    <t>IO_8fbddc5b-7ce3-4851-a14d-7194422dca44</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0938-0968</t>
+  </si>
+  <si>
+    <t>IO_8181a25d-c297-42d5-926e-117063d9fda6</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_0969-1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Hertfordshire and Buckinghamshire </t>
+  </si>
+  <si>
+    <t>IO_1ed63c75-f482-4508-a93b-841649cb6043</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1001-1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Buckinghamshire and Oxfordshire </t>
+  </si>
+  <si>
+    <t>IO_2903c96a-f8fe-4b2b-a469-923bc30c2f67</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1035-1071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Oxfordshire </t>
+  </si>
+  <si>
+    <t>IO_b5fa0e6b-d1f1-401a-a746-43de046856e1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1072-1106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Oxfordshire and Northamptonshire </t>
+  </si>
+  <si>
+    <t>IO_55a8edb8-cfbd-463e-84f0-a5d8f3aa2cc9</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1107-1137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Northamptonshire </t>
+  </si>
+  <si>
+    <t>IO_c9210de4-be40-4a5b-947f-aecab306d507</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1138-1169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Northamptonshire, Huntingdonshire and Bedfordshire </t>
+  </si>
+  <si>
+    <t>IO_d18cc560-6bd0-413a-8eb6-01c04d2989a9</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1170-1203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Bedfordshire and Cambridgeshire </t>
+  </si>
+  <si>
+    <t>IO_e08708e5-85d5-45ed-998f-5a294d446406</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1204-1238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Cambridgeshire and Essex </t>
+  </si>
+  <si>
+    <t>IO_fe892ead-bb06-419e-9409-b2a83aeb6e6e</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1239-1266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Essex </t>
+  </si>
+  <si>
+    <t>IO_4c61363e-d68b-4bf5-ace9-7fae1b6d9a0d</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1267-1304</t>
+  </si>
+  <si>
+    <t>IO_72076181-1ea6-4036-9fcd-5aa08dc87525</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1305-1344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Essex and Suffolk </t>
+  </si>
+  <si>
+    <t>IO_c5407d47-a2aa-4d48-8d1d-d0094f7bbb65</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1345-1376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Suffolk </t>
+  </si>
+  <si>
+    <t>IO_b7952eda-44c9-4369-9af2-b5881f57ba55</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1376-1417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Suffolk and Norfolk </t>
+  </si>
+  <si>
+    <t>IO_a0fa383c-efaf-46e2-b415-800322a104ef</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1418-1450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Norfolk </t>
+  </si>
+  <si>
+    <t>IO_2ccb43aa-b9b0-4b96-8b0f-b05b2cb7dbc1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1451-1477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Norfolk and Wiltshire </t>
+  </si>
+  <si>
+    <t>IO_5453673a-efa1-4241-9f70-478242ffe8bf</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1477-1504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Wiltshire </t>
+  </si>
+  <si>
+    <t>IO_6bd7f3e1-f360-4a4f-9575-85ebe2c16a1e</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1505-1537</t>
+  </si>
+  <si>
+    <t>IO_0500d818-b174-4d78-8884-50250454cd34</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1538-1567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Wiltshire and Dorset </t>
+  </si>
+  <si>
+    <t>IO_33cb123a-e7c7-46ba-858b-d28b09a4e845</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1568-1599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Dorset </t>
+  </si>
+  <si>
+    <t>IO_48323726-070c-4932-80dc-6f73b78009f1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1600-1628</t>
+  </si>
+  <si>
+    <t>IO_9061cb18-9846-4aae-84aa-231754ad9d20</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1629-1662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Dorset and Devon </t>
+  </si>
+  <si>
+    <t>IO_7af28698-dfa8-4ba4-a104-d9e67c3b19d6</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1663-1694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Devon </t>
+  </si>
+  <si>
+    <t>IO_747edd34-a7a2-4c63-baa6-54298a87b43c</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1695-1730</t>
+  </si>
+  <si>
+    <t>IO_b8f58d2c-11e5-4ffd-ae2e-c2993569674c</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1731-1753</t>
+  </si>
+  <si>
+    <t>IO_5f30e1d9-a993-498b-9459-9a5925f6a43d</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1754-1783</t>
+  </si>
+  <si>
+    <t>IO_24574359-9872-4387-8b7d-eca079ce3ed1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1784-1812</t>
+  </si>
+  <si>
+    <t>IO_3516965e-ffb9-4c54-8c87-70b64cfb17e0</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1813-1841</t>
+  </si>
+  <si>
+    <t>IO_fd8b207b-6aa1-4232-beca-cd10e1731bd8</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1842-1880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Devon and Cornwall </t>
+  </si>
+  <si>
+    <t>IO_eb3151ad-5761-4da6-a609-28ac642de31d</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1881-1911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Cornwall </t>
+  </si>
+  <si>
+    <t>IO_394581d0-6512-403c-9022-f4f01a65ff65</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2578-2612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Lincolnshire and Nottinghamshire </t>
+  </si>
+  <si>
+    <t>IO_a069f607-751b-477d-9c60-66244ccbb98f</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2613-2642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Nottinghamshire </t>
+  </si>
+  <si>
+    <t>IO_a8626505-ce8d-4be6-a176-32ee4e01a931</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2643-2660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Nottinghamshire and Derbyshire </t>
+  </si>
+  <si>
+    <t>IO_ea5d5dec-d8f0-413f-b7f5-001d14b298c5</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2661-2690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Derbyshire </t>
+  </si>
+  <si>
+    <t>IO_e264ffdd-dbc7-4a00-a952-52b6c38b6830</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2691-2727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Derbyshire and Cheshire </t>
+  </si>
+  <si>
+    <t>IO_0c9badb0-118d-4c5b-a975-776acdecb85c</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2728-2750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Cheshire </t>
+  </si>
+  <si>
+    <t>IO_98e74765-a5a2-4f30-a7ba-f6a61565b10c</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2751-2779</t>
+  </si>
+  <si>
+    <t>IO_a42a1236-1fc3-408c-8d3a-cea312b68a75</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2780-2815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Cheshire and Lancashire </t>
+  </si>
+  <si>
+    <t>IO_df0e2471-4139-49ca-981e-ba10224c54d7</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2816-2852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Lancashire </t>
+  </si>
+  <si>
+    <t>IO_ab2ece15-8b51-4a52-9b2f-5f2a1cc9872a</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2852-2900</t>
+  </si>
+  <si>
+    <t>IO_1bcbc2bf-4dc3-4ceb-9072-4579f3aa2249</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2901-2930</t>
+  </si>
+  <si>
+    <t>IO_37105d25-3931-451d-8084-4ec52d5998b6</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2931-2960</t>
+  </si>
+  <si>
+    <t>IO_9c6ce51a-bb8f-421a-8430-0e45e72a2ae4</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2961-2993</t>
+  </si>
+  <si>
+    <t>IO_9d852e10-977c-40ac-909e-4e8c57aece52</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2994-3024</t>
+  </si>
+  <si>
+    <t>IO_40b5ae17-9163-442a-9aee-b2f92052927e</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3025-3049</t>
+  </si>
+  <si>
+    <t>IO_3a815db2-0109-4e25-9fa1-eff7e6724f44</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3050-3087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Lancashire and Yorkshire </t>
+  </si>
+  <si>
+    <t>IO_6a02a5f8-68e0-4035-b314-1606ae5a7903</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3088-3116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Yorkshire </t>
+  </si>
+  <si>
+    <t>IO_66f8ae1d-8bdd-4017-b78e-8b6d2df58cbb</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3117-3138</t>
+  </si>
+  <si>
+    <t>IO_bdbf1a73-ef7c-481e-bf14-33d70b1314b4</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3139-3168</t>
+  </si>
+  <si>
+    <t>IO_3bb755f3-8544-423e-976d-6e12617065d8</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3169-3199</t>
+  </si>
+  <si>
+    <t>IO_f7223057-9f71-485e-805d-ac34af64205f</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3200-3242</t>
+  </si>
+  <si>
+    <t>IO_a017c2ac-5df5-4a81-8977-16127c947b9a</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3243-3283</t>
+  </si>
+  <si>
+    <t>IO_b6655ae4-0b00-46b0-881e-6a49d320d302</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3284-3324</t>
+  </si>
+  <si>
+    <t>IO_4a51e380-2ea6-4c10-8d5e-87c4712234f4</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3325-3365</t>
+  </si>
+  <si>
+    <t>IO_cf3e103b-f9cd-49e8-b3d2-ce12b15cc9be</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3366-3400</t>
+  </si>
+  <si>
+    <t>IO_6dd0d13b-109d-4b51-a17a-b54a686c1c21</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3401-3437</t>
+  </si>
+  <si>
+    <t>IO_873e2b57-0a36-47be-86b0-4bee4932e3e1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3438-3465</t>
+  </si>
+  <si>
+    <t>IO_f12f2c9b-d139-4136-b22f-023e73517250</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3466-3500</t>
+  </si>
+  <si>
+    <t>IO_def23689-0fd9-409e-9010-7d3c39dede86</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3501-3540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Durham </t>
+  </si>
+  <si>
+    <t>IO_f63f1036-131e-477c-a2f3-fb9e2eee1dad</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3540-3572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Durham and Northumberland </t>
+  </si>
+  <si>
+    <t>IO_8ab1836e-6733-4ce3-b927-3f3a86a9b723</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3573-3600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Northumberland </t>
+  </si>
+  <si>
+    <t>IO_6e9b65c5-38dd-4d04-b182-b0887b883b1e</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3601-3636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Northumberland and Cumberland </t>
+  </si>
+  <si>
+    <t>IO_19d90256-4126-4b25-8601-e0e9b9892d0f</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3637-3671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Cumberland and Westmorland </t>
+  </si>
+  <si>
+    <t>IO_ec2962c0-a2d8-4d3e-94d4-4a1065daf385</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3672-3700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Westmorland </t>
+  </si>
+  <si>
+    <t>IO_70696d38-053b-4de3-b1b9-d92bada4f104</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_3701-3730</t>
+  </si>
+  <si>
+    <t>IO_bdf58b47-8241-4e5f-884e-cc000f8b94b2</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4001-4032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Monmouthshire and Glamorganshire </t>
+  </si>
+  <si>
+    <t>IO_b24385f6-91ea-4adf-b578-ed5537d16ba8</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4033-4064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Glamorganshire </t>
+  </si>
+  <si>
+    <t>IO_88076c09-983a-4e85-9062-0614cb5227d1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4065-4091</t>
+  </si>
+  <si>
+    <t>IO_0e407497-8ae8-459e-aeb4-a714818c13e1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4092-4120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Glamorganshire, Carmathenshire and Pembrokeshire </t>
+  </si>
+  <si>
+    <t>IO_140fdad0-3863-45cb-b4cd-5d00ef0d07e3</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4121-4150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Pembrokeshire, Cardiganshire and Brecknockshire </t>
+  </si>
+  <si>
+    <t>IO_689bb402-0229-421a-90cb-b40d0fb31c65</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4151-4178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Brecknockshire </t>
+  </si>
+  <si>
+    <t>IO_0e910e68-529c-4310-8c16-7073f97f7b8f</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4179-4208</t>
+  </si>
+  <si>
+    <t>IO_d7e03e87-b723-4a30-b9e7-d48b48723bc6</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4209-4241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Brecknockshire and Radnorshire </t>
+  </si>
+  <si>
+    <t>IO_20331d6b-662d-492d-b8c8-9062ea5abaf1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4242-4269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Radnorshire, Montgomeryshire and Flintshire </t>
+  </si>
+  <si>
+    <t>IO_023788a1-c63e-4390-8db2-b2ddc0db7703</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4270-4300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Flintshire and Denbighshire </t>
+  </si>
+  <si>
+    <t>IO_41f7da5d-8e0e-4f25-a565-566e4966c0e1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4301-4327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Denbighshire and Merionethshire </t>
+  </si>
+  <si>
+    <t>IO_5584788b-97e2-45af-a5a9-31e266e89353</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4328-4360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Merionethshire and Caernavonshire </t>
+  </si>
+  <si>
+    <t>IO_d93d88d5-fe0a-4ef1-9c2a-4051c1aef7bd</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4361-4395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Caernavonshire </t>
+  </si>
+  <si>
+    <t>IO_aa9ba136-381b-41ce-8639-4820ee66a709</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4396-4432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Caernavonshire, Anglesey, Isle of Man and Channel Islands </t>
+  </si>
+  <si>
+    <t>IO_01220bf7-1421-4172-902d-f26cf5cf883a</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_4433-4446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Channel Islands </t>
+  </si>
+  <si>
+    <t>IO_31fee5f5-f8ab-4799-b0f2-982051d7ca92</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1912-1950</t>
+  </si>
+  <si>
+    <t>IO_d63af4c2-e47e-49ba-b503-7ebbdb44a8dc</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1951-1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Cornwall and Somerset </t>
+  </si>
+  <si>
+    <t>IO_e74117dd-9af5-4aa1-8e9e-da2d39b5f7fd</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_1987-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Somerset </t>
+  </si>
+  <si>
+    <t>IO_f0b13c47-b51d-47ec-a580-a26d8c0f001c</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2023-2056</t>
+  </si>
+  <si>
+    <t>IO_604667b5-e97f-418b-8db1-4cddf31cbe15</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2057-2087</t>
+  </si>
+  <si>
+    <t>IO_01964eae-5112-4fa3-a116-f15590c23ea8</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2088-2117</t>
+  </si>
+  <si>
+    <t>IO_4ca2002e-7602-4e8c-8300-ca871301b5b9</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2118-2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Somerset and Gloucestershire </t>
+  </si>
+  <si>
+    <t>IO_2ea6037c-0e6a-4dab-bfbe-7735c1ff56fd</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2151-2184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Gloucestershire </t>
+  </si>
+  <si>
+    <t>IO_a970b5e6-e003-43ad-9cba-ca305e89a290</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2185-2217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Gloucestershire and Herefordshire </t>
+  </si>
+  <si>
+    <t>IO_0dae52a2-af9d-4f98-abe6-7c2d54c2274f</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2218-2250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Herefordshire </t>
+  </si>
+  <si>
+    <t>IO_3f80355b-2069-4588-8936-61f1d7fe3b2b</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2251-2285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Herefordshire and Shropshire </t>
+  </si>
+  <si>
+    <t>IO_91d54eb8-38a6-4da1-a66e-9123227945a1</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2286-2325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Shropshire and Staffordshire </t>
+  </si>
+  <si>
+    <t>IO_448e1f50-d2de-4837-9a78-d4731b8e8eb3</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2326-2358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Staffordshire </t>
+  </si>
+  <si>
+    <t>IO_a2d3d62a-36fe-4209-a75a-b7dfe574186f</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2359-2396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Staffordshire and Worcestershire </t>
+  </si>
+  <si>
+    <t>IO_a808067b-3fef-4e2b-9f13-79ab9658dfd7</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2397-2438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Worcestershire </t>
+  </si>
+  <si>
+    <t>IO_a4cf4c8b-86c0-434f-bf89-116c54402b93</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2439-2450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Worcestershire and Warwickshire </t>
+  </si>
+  <si>
+    <t>IO_637fda62-9380-43da-a0cd-9d8784f22bcd</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2451-2488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Warwickshire </t>
+  </si>
+  <si>
+    <t>IO_f3e0e0f2-f781-4b1b-b9f9-3ae6c7d6a77a</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2489-2516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Warwickshire and Leicestershire </t>
+  </si>
+  <si>
+    <t>IO_fd8d55fa-d982-4739-a9b8-eb11cf8159c4</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2517-2543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Leicestershire and Lincolnshire </t>
+  </si>
+  <si>
+    <t>IO_8925730d-202b-422e-abfa-cd7832275fba</t>
+  </si>
+  <si>
+    <t>DRain_1931-1940_RainNos_2544-2578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1931-1940 daily rainfall for Lincolnshire </t>
   </si>
 </sst>
 </file>
@@ -3782,7 +4826,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5949EA17-9A17-41A4-8A1A-605F6AA36F9B}">
-  <dimension ref="A1:C393"/>
+  <dimension ref="A1:C523"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8119,8 +9163,1438 @@
         <v>945</v>
       </c>
     </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>946</v>
+      </c>
+      <c r="B394" t="s">
+        <v>947</v>
+      </c>
+      <c r="C394" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>949</v>
+      </c>
+      <c r="B395" t="s">
+        <v>950</v>
+      </c>
+      <c r="C395" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>952</v>
+      </c>
+      <c r="B396" t="s">
+        <v>953</v>
+      </c>
+      <c r="C396" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>955</v>
+      </c>
+      <c r="B397" t="s">
+        <v>956</v>
+      </c>
+      <c r="C397" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>957</v>
+      </c>
+      <c r="B398" t="s">
+        <v>958</v>
+      </c>
+      <c r="C398" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>959</v>
+      </c>
+      <c r="B399" t="s">
+        <v>960</v>
+      </c>
+      <c r="C399" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>961</v>
+      </c>
+      <c r="B400" t="s">
+        <v>962</v>
+      </c>
+      <c r="C400" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>963</v>
+      </c>
+      <c r="B401" t="s">
+        <v>964</v>
+      </c>
+      <c r="C401" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>965</v>
+      </c>
+      <c r="B402" t="s">
+        <v>966</v>
+      </c>
+      <c r="C402" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>968</v>
+      </c>
+      <c r="B403" t="s">
+        <v>969</v>
+      </c>
+      <c r="C403" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>971</v>
+      </c>
+      <c r="B404" t="s">
+        <v>972</v>
+      </c>
+      <c r="C404" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>973</v>
+      </c>
+      <c r="B405" t="s">
+        <v>974</v>
+      </c>
+      <c r="C405" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>975</v>
+      </c>
+      <c r="B406" t="s">
+        <v>976</v>
+      </c>
+      <c r="C406" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>977</v>
+      </c>
+      <c r="B407" t="s">
+        <v>978</v>
+      </c>
+      <c r="C407" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>980</v>
+      </c>
+      <c r="B408" t="s">
+        <v>981</v>
+      </c>
+      <c r="C408" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>983</v>
+      </c>
+      <c r="B409" t="s">
+        <v>984</v>
+      </c>
+      <c r="C409" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>985</v>
+      </c>
+      <c r="B410" t="s">
+        <v>986</v>
+      </c>
+      <c r="C410" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>987</v>
+      </c>
+      <c r="B411" t="s">
+        <v>988</v>
+      </c>
+      <c r="C411" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>989</v>
+      </c>
+      <c r="B412" t="s">
+        <v>990</v>
+      </c>
+      <c r="C412" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>991</v>
+      </c>
+      <c r="B413" t="s">
+        <v>992</v>
+      </c>
+      <c r="C413" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>994</v>
+      </c>
+      <c r="B414" t="s">
+        <v>995</v>
+      </c>
+      <c r="C414" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>997</v>
+      </c>
+      <c r="B415" t="s">
+        <v>998</v>
+      </c>
+      <c r="C415" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>999</v>
+      </c>
+      <c r="B416" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C416" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B417" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C417" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B418" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C418" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C419" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C420" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C421" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C422" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B423" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C423" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B424" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C424" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B425" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C425" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C426" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B427" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C427" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B428" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C428" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B429" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C429" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B430" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C430" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C431" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C432" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B433" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C433" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B434" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C434" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C435" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B436" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C436" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B437" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C437" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B438" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C438" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B439" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C439" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B440" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C440" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B441" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C441" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C442" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C443" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C444" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C445" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B446" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C446" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B447" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C447" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B448" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C448" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B449" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C449" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B450" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C450" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B451" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C451" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B452" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C452" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B453" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C453" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B454" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C454" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B455" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C455" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C456" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B457" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C457" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B458" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C458" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B459" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C459" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B460" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C460" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B461" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C461" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B462" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C462" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B463" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C463" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B464" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C464" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B465" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C465" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C466" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B467" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C467" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B468" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C468" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B469" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C469" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B470" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C470" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B471" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C471" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B472" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C472" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B473" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C473" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B474" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C474" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B475" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C475" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B476" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C476" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B477" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C477" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B478" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C478" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B479" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C479" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B480" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C480" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B481" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C481" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B482" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C482" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B483" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C483" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B484" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C484" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B485" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C485" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B486" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C486" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B487" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C487" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B488" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C488" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B489" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C489" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B490" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C490" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B491" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C491" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B492" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C492" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C493" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B494" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C494" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C496" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B497" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C497" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B498" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C498" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B499" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C499" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C500" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C501" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B502" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C502" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C503" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C504" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C505" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C506" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B507" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C507" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B508" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C508" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B509" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C509" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B510" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C510" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B511" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C511" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B512" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C512" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B513" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C513" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C514" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C515" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B516" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C516" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B517" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C517" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B518" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C518" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B519" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C519" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B520" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C520" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B521" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C521" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B522" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C522" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B523" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C523" t="s">
+        <v>1285</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C241" xr:uid="{5949EA17-9A17-41A4-8A1A-605F6AA36F9B}"/>
+  <autoFilter ref="A1:C523" xr:uid="{5949EA17-9A17-41A4-8A1A-605F6AA36F9B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>